<commit_message>
* bug fix : add Format#get_alignment_key. typo in Styles#write_xf. test pass!
</commit_message>
<xml_diff>
--- a/test/perl_output/indent.xlsx
+++ b/test/perl_output/indent.xlsx
@@ -55,10 +55,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -369,7 +372,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>